<commit_message>
completed the first exercice of the project
one more to go
</commit_message>
<xml_diff>
--- a/Finals Project/data/exercice1.xlsx
+++ b/Finals Project/data/exercice1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\License Big Data\Semester 5\Techniques de prevision\notebooks\Finals Project\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3324F24A-F30C-4269-81AB-4DCF1213961F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="6855" windowHeight="4380"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -93,8 +99,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,11 +137,52 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ACBA416D-6155-49E0-9325-0A4168575C9A}" name="Table1" displayName="Table1" ref="A1:X92" totalsRowShown="0">
+  <autoFilter ref="A1:X92" xr:uid="{ACBA416D-6155-49E0-9325-0A4168575C9A}"/>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{2E9CE56C-3B5E-4CF0-80B9-33D386EEEE4E}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{805A4DAD-2467-45AF-825D-E4F0841AD313}" name="sexe"/>
+    <tableColumn id="3" xr3:uid="{0AA46EFD-0E35-4A51-934F-BC710B1D7E71}" name="Region"/>
+    <tableColumn id="4" xr3:uid="{D41AA406-2AA8-48B0-A872-339E69EDB3C3}" name="Age"/>
+    <tableColumn id="5" xr3:uid="{064F40CF-2752-47E8-9EF4-87EC9121E0BD}" name="etat_civil"/>
+    <tableColumn id="6" xr3:uid="{387971B4-561D-48BF-B1B8-2AF39F9B3366}" name="N_educatif"/>
+    <tableColumn id="7" xr3:uid="{5FB20D41-0796-4806-99B2-72C686DFCA64}" name="Membre_famille"/>
+    <tableColumn id="8" xr3:uid="{8FB1518F-4E75-42FC-A061-E1C77D4B4404}" name="Revenu_famille"/>
+    <tableColumn id="9" xr3:uid="{F35BA5A8-7162-480F-BADF-88895F3CE3F3}" name="Revenu_Mensuelle"/>
+    <tableColumn id="10" xr3:uid="{766A7605-2709-48B1-AC1C-9467456BD762}" name="Redoublant"/>
+    <tableColumn id="11" xr3:uid="{9E2A5837-87E5-4783-BD67-C58CC44BEB3C}" name="Prob_Enseignat"/>
+    <tableColumn id="12" xr3:uid="{31B106BF-336F-41C1-B904-476876B0202D}" name="Aide_ecole"/>
+    <tableColumn id="13" xr3:uid="{8C496485-A6FD-46B3-9094-CEC56F865A2C}" name="Rq_Comprtement"/>
+    <tableColumn id="14" xr3:uid="{F5A7590E-11CE-4CF3-BCB4-4FF9DAFB21DC}" name="Relat_Parent"/>
+    <tableColumn id="15" xr3:uid="{CB71DE26-C7EB-4158-AB09-AE6D9879CCA3}" name="Niveau_educ_pere"/>
+    <tableColumn id="16" xr3:uid="{AFF4846A-5363-4FF0-87C9-2A023FDC0EFB}" name="Niveau_educ_mere"/>
+    <tableColumn id="17" xr3:uid="{4DBBC82B-1EF9-4C00-9355-6FC0E93503C1}" name="Sign_ecole"/>
+    <tableColumn id="18" xr3:uid="{990CDECC-1CFE-4B5E-8BEA-010E42E545CE}" name="Endroit_freq"/>
+    <tableColumn id="19" xr3:uid="{DC5ED6BC-8445-46BC-AD11-3B333EA1FCEA}" name="Ph_famille"/>
+    <tableColumn id="20" xr3:uid="{6F6E5F4F-4333-4237-A6F5-AA07D674A0E2}" name="Ricule_Prof"/>
+    <tableColumn id="21" xr3:uid="{2ED099E3-3C3F-4277-BDB4-397BB04E2C29}" name="Ricule_collegue"/>
+    <tableColumn id="22" xr3:uid="{24A2E698-EBF8-41AD-90B5-8B4E7815B920}" name="Sensation_apres_ecole"/>
+    <tableColumn id="23" xr3:uid="{EECAD3EC-9A97-481A-BAA4-70BD1817FE06}" name="Apres_repture_ecole"/>
+    <tableColumn id="24" xr3:uid="{8079D1BA-3FD5-4455-9D2C-51D0E77466C9}" name="Violence"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -177,7 +224,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -209,9 +256,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -243,6 +308,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -418,16 +501,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1"/>
+    <col min="16" max="16" width="19.21875" customWidth="1"/>
+    <col min="17" max="17" width="11.88671875" customWidth="1"/>
+    <col min="18" max="18" width="13.44140625" customWidth="1"/>
+    <col min="19" max="19" width="11.77734375" customWidth="1"/>
+    <col min="20" max="20" width="12.44140625" customWidth="1"/>
+    <col min="21" max="21" width="15.88671875" customWidth="1"/>
+    <col min="22" max="22" width="22.109375" customWidth="1"/>
+    <col min="23" max="23" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +604,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -575,7 +678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -649,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -723,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -797,7 +900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -871,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>9</v>
       </c>
@@ -945,7 +1048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1019,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>11</v>
       </c>
@@ -1093,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>12</v>
       </c>
@@ -1167,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>15</v>
       </c>
@@ -1241,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>16</v>
       </c>
@@ -1315,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>17</v>
       </c>
@@ -1389,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>19</v>
       </c>
@@ -1463,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>20</v>
       </c>
@@ -1537,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>21</v>
       </c>
@@ -1611,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>22</v>
       </c>
@@ -1685,7 +1788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>23</v>
       </c>
@@ -1759,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>24</v>
       </c>
@@ -1833,7 +1936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>25</v>
       </c>
@@ -1907,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>26</v>
       </c>
@@ -1981,7 +2084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>27</v>
       </c>
@@ -2055,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>28</v>
       </c>
@@ -2129,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>29</v>
       </c>
@@ -2203,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>31</v>
       </c>
@@ -2277,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>32</v>
       </c>
@@ -2351,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>34</v>
       </c>
@@ -2425,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>35</v>
       </c>
@@ -2499,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>36</v>
       </c>
@@ -2573,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>37</v>
       </c>
@@ -2647,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>38</v>
       </c>
@@ -2721,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>39</v>
       </c>
@@ -2795,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>40</v>
       </c>
@@ -2869,7 +2972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>41</v>
       </c>
@@ -2943,7 +3046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>43</v>
       </c>
@@ -3014,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>44</v>
       </c>
@@ -3088,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>46</v>
       </c>
@@ -3162,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:24">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>50</v>
       </c>
@@ -3236,7 +3339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>51</v>
       </c>
@@ -3310,7 +3413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>52</v>
       </c>
@@ -3384,7 +3487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:24">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>54</v>
       </c>
@@ -3458,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>55</v>
       </c>
@@ -3532,7 +3635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:24">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>57</v>
       </c>
@@ -3606,7 +3709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:24">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>58</v>
       </c>
@@ -3680,7 +3783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:24">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>60</v>
       </c>
@@ -3754,7 +3857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:24">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>62</v>
       </c>
@@ -3828,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:24">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>64</v>
       </c>
@@ -3902,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>65</v>
       </c>
@@ -3976,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>67</v>
       </c>
@@ -4050,7 +4153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>68</v>
       </c>
@@ -4124,7 +4227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>70</v>
       </c>
@@ -4198,7 +4301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>72</v>
       </c>
@@ -4272,7 +4375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>75</v>
       </c>
@@ -4346,7 +4449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>76</v>
       </c>
@@ -4420,7 +4523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>78</v>
       </c>
@@ -4494,7 +4597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>79</v>
       </c>
@@ -4568,7 +4671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>80</v>
       </c>
@@ -4642,7 +4745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>81</v>
       </c>
@@ -4716,7 +4819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>83</v>
       </c>
@@ -4790,7 +4893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:24">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>85</v>
       </c>
@@ -4864,7 +4967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>87</v>
       </c>
@@ -4938,7 +5041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>88</v>
       </c>
@@ -5012,7 +5115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>90</v>
       </c>
@@ -5086,7 +5189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>91</v>
       </c>
@@ -5160,7 +5263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:24">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>92</v>
       </c>
@@ -5234,7 +5337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:24">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>95</v>
       </c>
@@ -5308,7 +5411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:24">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>96</v>
       </c>
@@ -5382,7 +5485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:24">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>97</v>
       </c>
@@ -5456,7 +5559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:24">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>105</v>
       </c>
@@ -5530,7 +5633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:24">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>106</v>
       </c>
@@ -5604,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:24">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>107</v>
       </c>
@@ -5678,7 +5781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:24">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>108</v>
       </c>
@@ -5752,7 +5855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:24">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>109</v>
       </c>
@@ -5826,7 +5929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:24">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>111</v>
       </c>
@@ -5900,7 +6003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:24">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>113</v>
       </c>
@@ -5974,7 +6077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:24">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>114</v>
       </c>
@@ -6048,7 +6151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:24">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>115</v>
       </c>
@@ -6122,7 +6225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:24">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>117</v>
       </c>
@@ -6196,7 +6299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:24">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>122</v>
       </c>
@@ -6270,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:24">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>124</v>
       </c>
@@ -6344,7 +6447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:24">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>135</v>
       </c>
@@ -6418,7 +6521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:24">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>136</v>
       </c>
@@ -6492,7 +6595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:24">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>137</v>
       </c>
@@ -6566,7 +6669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:24">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>138</v>
       </c>
@@ -6640,7 +6743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:24">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>139</v>
       </c>
@@ -6714,7 +6817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:24">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>140</v>
       </c>
@@ -6788,7 +6891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:24">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>141</v>
       </c>
@@ -6862,7 +6965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:24">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>143</v>
       </c>
@@ -6936,7 +7039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:24">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>144</v>
       </c>
@@ -7010,7 +7113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:24">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>145</v>
       </c>
@@ -7084,7 +7187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:24">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>147</v>
       </c>
@@ -7158,7 +7261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:24">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>148</v>
       </c>
@@ -7234,28 +7337,31 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>